<commit_message>
remove the other volatiles (from stem trichomes)
</commit_message>
<xml_diff>
--- a/TableS4_Kovats_calculations/Retention_Index_Calculation_ramp_5_10_KOVATS-qTOF.xlsx
+++ b/TableS4_Kovats_calculations/Retention_Index_Calculation_ramp_5_10_KOVATS-qTOF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgalland/Documents/workspace/natural-insecticides-machine-learning-paper/TableS4_Kovats_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA49B24-9493-914D-B3A8-927A9FCD1A93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2237D2D1-BCD2-EC41-BD10-8D42A678EFF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4540" yWindow="1280" windowWidth="42240" windowHeight="24620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>n-nonane</t>
   </si>
@@ -452,7 +452,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E946016D-57B2-654F-ACAE-29754D674E85}">
   <dimension ref="A1:XFD90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38:F55"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1453,7 +1453,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="17">
-        <f t="shared" ref="B39:B55" si="3">K41*60</f>
+        <f t="shared" ref="B41:B55" si="3">K41*60</f>
         <v>1482.42</v>
       </c>
       <c r="C41" s="14">
@@ -1879,48 +1879,30 @@
       </c>
     </row>
     <row r="59" spans="1:16384" x14ac:dyDescent="0.15">
-      <c r="A59" s="37">
-        <v>4.12</v>
-      </c>
+      <c r="A59" s="37"/>
       <c r="B59" s="31"/>
       <c r="C59" s="32"/>
       <c r="D59" s="32"/>
-      <c r="E59" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F59" s="32" t="s">
-        <v>45</v>
-      </c>
+      <c r="E59" s="32"/>
+      <c r="F59" s="32"/>
       <c r="G59" s="12"/>
     </row>
     <row r="60" spans="1:16384" x14ac:dyDescent="0.15">
-      <c r="A60" s="37">
-        <v>4.7699999999999996</v>
-      </c>
+      <c r="A60" s="37"/>
       <c r="B60" s="31"/>
       <c r="C60" s="32"/>
       <c r="D60" s="32"/>
-      <c r="E60" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F60" s="32" t="s">
-        <v>45</v>
-      </c>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
       <c r="G60" s="12"/>
     </row>
     <row r="61" spans="1:16384" x14ac:dyDescent="0.15">
-      <c r="A61" s="38">
-        <v>5.35</v>
-      </c>
+      <c r="A61" s="38"/>
       <c r="B61" s="31"/>
       <c r="C61" s="32"/>
       <c r="D61" s="32"/>
-      <c r="E61" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F61" s="32" t="s">
-        <v>45</v>
-      </c>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -18301,18 +18283,12 @@
       <c r="XFD61" s="4"/>
     </row>
     <row r="62" spans="1:16384" x14ac:dyDescent="0.15">
-      <c r="A62" s="38">
-        <v>5.65</v>
-      </c>
+      <c r="A62" s="38"/>
       <c r="B62" s="31"/>
       <c r="C62" s="32"/>
       <c r="D62" s="32"/>
-      <c r="E62" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F62" s="32" t="s">
-        <v>45</v>
-      </c>
+      <c r="E62" s="32"/>
+      <c r="F62" s="32"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
@@ -34693,18 +34669,12 @@
       <c r="XFD62" s="4"/>
     </row>
     <row r="63" spans="1:16384" x14ac:dyDescent="0.15">
-      <c r="A63" s="38">
-        <v>7.33</v>
-      </c>
+      <c r="A63" s="38"/>
       <c r="B63" s="31"/>
       <c r="C63" s="32"/>
       <c r="D63" s="32"/>
-      <c r="E63" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F63" s="32" t="s">
-        <v>45</v>
-      </c>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
@@ -51085,18 +51055,12 @@
       <c r="XFD63" s="4"/>
     </row>
     <row r="64" spans="1:16384" x14ac:dyDescent="0.15">
-      <c r="A64" s="38">
-        <v>7.62</v>
-      </c>
+      <c r="A64" s="38"/>
       <c r="B64" s="31"/>
       <c r="C64" s="32"/>
       <c r="D64" s="32"/>
-      <c r="E64" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F64" s="32" t="s">
-        <v>45</v>
-      </c>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
@@ -67477,424 +67441,218 @@
       <c r="XFD64" s="4"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A65" s="33">
-        <f>B65/60</f>
-        <v>0</v>
-      </c>
+      <c r="A65" s="33"/>
       <c r="B65" s="34"/>
       <c r="C65" s="32"/>
       <c r="D65" s="32"/>
-      <c r="E65" s="35">
-        <v>9</v>
-      </c>
-      <c r="F65" s="35" t="e">
-        <f>100*E65+100*((B65-C65)/(D65-C65))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E65" s="35"/>
+      <c r="F65" s="35"/>
       <c r="G65" s="13"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A66" s="33">
-        <f t="shared" ref="A66:A90" si="5">B66/60</f>
-        <v>0</v>
-      </c>
+      <c r="A66" s="33"/>
       <c r="B66" s="34"/>
       <c r="C66" s="32"/>
       <c r="D66" s="32"/>
-      <c r="E66" s="35">
-        <v>9</v>
-      </c>
-      <c r="F66" s="35" t="e">
-        <f>100*E66+100*((B66-C66)/(D66-C66))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E66" s="35"/>
+      <c r="F66" s="35"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A67" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A67" s="33"/>
       <c r="B67" s="33"/>
       <c r="C67" s="32"/>
       <c r="D67" s="32"/>
-      <c r="E67" s="35">
-        <v>9</v>
-      </c>
-      <c r="F67" s="35" t="e">
-        <f t="shared" ref="F67:F88" si="6">100*E67+100*((B67-C67)/(D67-C67))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E67" s="35"/>
+      <c r="F67" s="35"/>
       <c r="G67" s="13"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A68" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A68" s="33"/>
       <c r="B68" s="33"/>
       <c r="C68" s="32"/>
       <c r="D68" s="32"/>
-      <c r="E68" s="35">
-        <v>9</v>
-      </c>
-      <c r="F68" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E68" s="35"/>
+      <c r="F68" s="35"/>
       <c r="G68" s="13"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A69" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A69" s="33"/>
       <c r="B69" s="34"/>
       <c r="C69" s="36"/>
       <c r="D69" s="34"/>
-      <c r="E69" s="35">
-        <v>10</v>
-      </c>
-      <c r="F69" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E69" s="35"/>
+      <c r="F69" s="35"/>
       <c r="G69" s="13"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A70" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A70" s="33"/>
       <c r="B70" s="34"/>
       <c r="C70" s="36"/>
       <c r="D70" s="34"/>
-      <c r="E70" s="35">
-        <v>10</v>
-      </c>
-      <c r="F70" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E70" s="35"/>
+      <c r="F70" s="35"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A71" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A71" s="33"/>
       <c r="B71" s="34"/>
       <c r="C71" s="36"/>
       <c r="D71" s="34"/>
-      <c r="E71" s="35">
-        <v>10</v>
-      </c>
-      <c r="F71" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E71" s="35"/>
+      <c r="F71" s="35"/>
       <c r="G71" s="13"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A72" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A72" s="33"/>
       <c r="B72" s="34"/>
       <c r="C72" s="36"/>
       <c r="D72" s="34"/>
-      <c r="E72" s="35">
-        <v>10</v>
-      </c>
-      <c r="F72" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E72" s="35"/>
+      <c r="F72" s="35"/>
       <c r="G72" s="13"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A73" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A73" s="33"/>
       <c r="B73" s="34"/>
       <c r="C73" s="36"/>
       <c r="D73" s="34"/>
-      <c r="E73" s="35">
-        <v>13</v>
-      </c>
-      <c r="F73" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E73" s="35"/>
+      <c r="F73" s="35"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A74" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A74" s="33"/>
       <c r="B74" s="34"/>
       <c r="C74" s="36"/>
       <c r="D74" s="34"/>
-      <c r="E74" s="35">
-        <v>13</v>
-      </c>
-      <c r="F74" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E74" s="35"/>
+      <c r="F74" s="35"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A75" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A75" s="33"/>
       <c r="B75" s="34"/>
       <c r="C75" s="36"/>
       <c r="D75" s="34"/>
-      <c r="E75" s="35">
-        <v>14</v>
-      </c>
-      <c r="F75" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E75" s="35"/>
+      <c r="F75" s="35"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A76" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A76" s="33"/>
       <c r="B76" s="34"/>
       <c r="C76" s="36"/>
       <c r="D76" s="34"/>
-      <c r="E76" s="35">
-        <v>14</v>
-      </c>
-      <c r="F76" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E76" s="35"/>
+      <c r="F76" s="35"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A77" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A77" s="33"/>
       <c r="B77" s="34"/>
       <c r="C77" s="36"/>
       <c r="D77" s="34"/>
-      <c r="E77" s="35">
-        <v>14</v>
-      </c>
-      <c r="F77" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E77" s="35"/>
+      <c r="F77" s="35"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A78" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A78" s="33"/>
       <c r="B78" s="34"/>
       <c r="C78" s="36"/>
       <c r="D78" s="34"/>
-      <c r="E78" s="35">
-        <v>14</v>
-      </c>
-      <c r="F78" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E78" s="35"/>
+      <c r="F78" s="35"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A79" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A79" s="33"/>
       <c r="B79" s="34"/>
       <c r="C79" s="36"/>
       <c r="D79" s="34"/>
-      <c r="E79" s="35">
-        <v>14</v>
-      </c>
-      <c r="F79" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E79" s="35"/>
+      <c r="F79" s="35"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A80" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A80" s="33"/>
       <c r="B80" s="34"/>
       <c r="C80" s="36"/>
       <c r="D80" s="34"/>
-      <c r="E80" s="35">
-        <v>15</v>
-      </c>
-      <c r="F80" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E80" s="35"/>
+      <c r="F80" s="35"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A81" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A81" s="33"/>
       <c r="B81" s="34"/>
       <c r="C81" s="36"/>
       <c r="D81" s="34"/>
-      <c r="E81" s="35">
-        <v>15</v>
-      </c>
-      <c r="F81" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E81" s="35"/>
+      <c r="F81" s="35"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A82" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A82" s="33"/>
       <c r="B82" s="34"/>
       <c r="C82" s="36"/>
       <c r="D82" s="34"/>
-      <c r="E82" s="35">
-        <v>15</v>
-      </c>
-      <c r="F82" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E82" s="35"/>
+      <c r="F82" s="35"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A83" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A83" s="33"/>
       <c r="B83" s="34"/>
       <c r="C83" s="36"/>
       <c r="D83" s="34"/>
-      <c r="E83" s="35">
-        <v>15</v>
-      </c>
-      <c r="F83" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E83" s="35"/>
+      <c r="F83" s="35"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A84" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A84" s="33"/>
       <c r="B84" s="34"/>
       <c r="C84" s="36"/>
       <c r="D84" s="34"/>
-      <c r="E84" s="35">
-        <v>15</v>
-      </c>
-      <c r="F84" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E84" s="35"/>
+      <c r="F84" s="35"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A85" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A85" s="33"/>
       <c r="B85" s="34"/>
       <c r="C85" s="36"/>
       <c r="D85" s="34"/>
-      <c r="E85" s="35">
-        <v>16</v>
-      </c>
-      <c r="F85" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E85" s="35"/>
+      <c r="F85" s="35"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A86" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A86" s="33"/>
       <c r="B86" s="34"/>
       <c r="C86" s="36"/>
       <c r="D86" s="34"/>
-      <c r="E86" s="35">
-        <v>16</v>
-      </c>
-      <c r="F86" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E86" s="35"/>
+      <c r="F86" s="35"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A87" s="33">
-        <f>B87/60</f>
-        <v>0</v>
-      </c>
+      <c r="A87" s="33"/>
       <c r="B87" s="34"/>
       <c r="C87" s="36"/>
       <c r="D87" s="34"/>
-      <c r="E87" s="35">
-        <v>17</v>
-      </c>
-      <c r="F87" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E87" s="35"/>
+      <c r="F87" s="35"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A88" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A88" s="33"/>
       <c r="B88" s="34"/>
       <c r="C88" s="36"/>
       <c r="D88" s="34"/>
-      <c r="E88" s="35">
-        <v>19</v>
-      </c>
-      <c r="F88" s="35" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E88" s="35"/>
+      <c r="F88" s="35"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A89" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A89" s="33"/>
       <c r="B89" s="34"/>
       <c r="C89" s="36"/>
       <c r="D89" s="36"/>
-      <c r="E89" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="F89" s="36" t="s">
-        <v>45</v>
-      </c>
+      <c r="E89" s="36"/>
+      <c r="F89" s="36"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A90" s="33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="A90" s="33"/>
       <c r="B90" s="34"/>
       <c r="C90" s="36"/>
       <c r="D90" s="36"/>
-      <c r="E90" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="F90" s="36" t="s">
-        <v>45</v>
-      </c>
+      <c r="E90" s="36"/>
+      <c r="F90" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>